<commit_message>
Fix institution code handling in RDF graph creation; update location dictionary key to use institution code.
</commit_message>
<xml_diff>
--- a/docs/Localizacao.xlsx
+++ b/docs/Localizacao.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joana\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fcul\RC\Trabalho\knowledge-graph-to-higher-education-pt\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8A43A8-9A6E-4033-B524-1DF968FC9D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F43E1B-3BE5-4B2D-9E95-2F187FDA1FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9C0474DA-C869-4094-B24B-FF17B07AFA22}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1884" uniqueCount="1071">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1885" uniqueCount="1071">
   <si>
     <t>Código do Estabelecimento</t>
   </si>
@@ -3273,10 +3273,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3593,8 +3592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94BEAACD-A4C7-4CEB-A179-BFE0F5FD2720}">
   <dimension ref="A1:M207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
-      <selection activeCell="J207" sqref="J207"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H184" sqref="H184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7759,7 +7758,7 @@
       <c r="I105" t="s">
         <v>17</v>
       </c>
-      <c r="J105" s="2" t="s">
+      <c r="J105" t="s">
         <v>739</v>
       </c>
       <c r="K105" t="s">
@@ -9166,7 +9165,7 @@
       <c r="I141" t="s">
         <v>50</v>
       </c>
-      <c r="J141" s="2" t="s">
+      <c r="J141" t="s">
         <v>781</v>
       </c>
       <c r="K141" t="s">
@@ -9207,7 +9206,7 @@
       <c r="I142" t="s">
         <v>50</v>
       </c>
-      <c r="J142" s="2" t="s">
+      <c r="J142" t="s">
         <v>769</v>
       </c>
       <c r="K142" t="s">
@@ -9248,7 +9247,7 @@
       <c r="I143" t="s">
         <v>50</v>
       </c>
-      <c r="J143" s="2" t="s">
+      <c r="J143" t="s">
         <v>776</v>
       </c>
       <c r="K143" t="s">
@@ -9289,7 +9288,7 @@
       <c r="I144" t="s">
         <v>50</v>
       </c>
-      <c r="J144" s="2" t="s">
+      <c r="J144" t="s">
         <v>770</v>
       </c>
       <c r="K144" t="s">
@@ -9330,7 +9329,7 @@
       <c r="I145" t="s">
         <v>50</v>
       </c>
-      <c r="J145" s="2" t="s">
+      <c r="J145" t="s">
         <v>773</v>
       </c>
       <c r="K145" t="s">
@@ -9371,7 +9370,7 @@
       <c r="I146" t="s">
         <v>50</v>
       </c>
-      <c r="J146" s="2" t="s">
+      <c r="J146" t="s">
         <v>783</v>
       </c>
       <c r="K146" t="s">
@@ -9412,7 +9411,7 @@
       <c r="I147" t="s">
         <v>50</v>
       </c>
-      <c r="J147" s="2" t="s">
+      <c r="J147" t="s">
         <v>785</v>
       </c>
       <c r="K147" t="s">
@@ -9453,7 +9452,7 @@
       <c r="I148" t="s">
         <v>50</v>
       </c>
-      <c r="J148" s="2" t="s">
+      <c r="J148" t="s">
         <v>789</v>
       </c>
       <c r="K148" t="s">
@@ -9494,7 +9493,7 @@
       <c r="I149" t="s">
         <v>50</v>
       </c>
-      <c r="J149" s="2" t="s">
+      <c r="J149" t="s">
         <v>797</v>
       </c>
       <c r="K149" t="s">
@@ -9535,7 +9534,7 @@
       <c r="I150" t="s">
         <v>50</v>
       </c>
-      <c r="J150" s="2" t="s">
+      <c r="J150" t="s">
         <v>802</v>
       </c>
       <c r="K150" t="s">
@@ -9576,7 +9575,7 @@
       <c r="I151" t="s">
         <v>50</v>
       </c>
-      <c r="J151" s="2" t="s">
+      <c r="J151" t="s">
         <v>791</v>
       </c>
       <c r="K151" t="s">
@@ -9617,7 +9616,7 @@
       <c r="I152" t="s">
         <v>50</v>
       </c>
-      <c r="J152" s="2" t="s">
+      <c r="J152" t="s">
         <v>804</v>
       </c>
       <c r="K152" t="s">
@@ -9699,7 +9698,7 @@
       <c r="I154" t="s">
         <v>50</v>
       </c>
-      <c r="J154" s="2" t="s">
+      <c r="J154" t="s">
         <v>812</v>
       </c>
       <c r="K154" t="s">
@@ -9740,7 +9739,7 @@
       <c r="I155" t="s">
         <v>50</v>
       </c>
-      <c r="J155" s="2" t="s">
+      <c r="J155" t="s">
         <v>817</v>
       </c>
       <c r="K155" t="s">
@@ -10176,7 +10175,7 @@
       <c r="I166" t="s">
         <v>50</v>
       </c>
-      <c r="J166" s="2" t="s">
+      <c r="J166" t="s">
         <v>875</v>
       </c>
       <c r="K166" t="s">
@@ -10454,7 +10453,7 @@
       <c r="I173" t="s">
         <v>50</v>
       </c>
-      <c r="J173" s="2" t="s">
+      <c r="J173" t="s">
         <v>911</v>
       </c>
       <c r="K173" t="s">
@@ -10495,7 +10494,7 @@
       <c r="I174" t="s">
         <v>17</v>
       </c>
-      <c r="J174" s="2" t="s">
+      <c r="J174" t="s">
         <v>948</v>
       </c>
       <c r="K174" t="s">
@@ -10536,7 +10535,7 @@
       <c r="I175" t="s">
         <v>17</v>
       </c>
-      <c r="J175" s="2" t="s">
+      <c r="J175" t="s">
         <v>949</v>
       </c>
       <c r="K175" t="s">
@@ -10577,7 +10576,7 @@
       <c r="I176" t="s">
         <v>17</v>
       </c>
-      <c r="J176" s="2" t="s">
+      <c r="J176" t="s">
         <v>949</v>
       </c>
       <c r="K176" t="s">
@@ -10618,7 +10617,7 @@
       <c r="I177" t="s">
         <v>17</v>
       </c>
-      <c r="J177" s="2" t="s">
+      <c r="J177" t="s">
         <v>950</v>
       </c>
       <c r="K177" t="s">
@@ -10659,7 +10658,7 @@
       <c r="I178" t="s">
         <v>50</v>
       </c>
-      <c r="J178" s="2" t="s">
+      <c r="J178" t="s">
         <v>945</v>
       </c>
       <c r="K178" t="s">
@@ -10700,7 +10699,7 @@
       <c r="I179" t="s">
         <v>50</v>
       </c>
-      <c r="J179" s="2" t="s">
+      <c r="J179" t="s">
         <v>946</v>
       </c>
       <c r="K179" t="s">
@@ -10741,7 +10740,7 @@
       <c r="I180" t="s">
         <v>50</v>
       </c>
-      <c r="J180" s="2" t="s">
+      <c r="J180" t="s">
         <v>947</v>
       </c>
       <c r="K180" t="s">
@@ -10782,7 +10781,7 @@
       <c r="I181" t="s">
         <v>17</v>
       </c>
-      <c r="J181" s="2" t="s">
+      <c r="J181" t="s">
         <v>951</v>
       </c>
       <c r="K181" t="s">
@@ -10889,6 +10888,9 @@
       </c>
       <c r="G184" t="s">
         <v>476</v>
+      </c>
+      <c r="H184" t="s">
+        <v>955</v>
       </c>
       <c r="I184" t="s">
         <v>17</v>

</xml_diff>